<commit_message>
Sua mensagem de commit aqui
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\OneDrive\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BD8389-C504-4D51-AFCD-341372082340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88704054-E073-47BB-8B1F-A6C4E443ADAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -42,16 +31,16 @@
     <t>Acompanhamento</t>
   </si>
   <si>
-    <t>carne</t>
-  </si>
-  <si>
-    <t>frango</t>
-  </si>
-  <si>
-    <t>peixe</t>
-  </si>
-  <si>
-    <t>vegetariana</t>
+    <t>Aves</t>
+  </si>
+  <si>
+    <t>Peixes</t>
+  </si>
+  <si>
+    <t>Bovino</t>
+  </si>
+  <si>
+    <t>Suino</t>
   </si>
   <si>
     <t>pequena</t>
@@ -376,7 +365,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,14 +375,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -436,12 +417,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,20 +726,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H236"/>
+  <dimension ref="A1:C236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -781,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -792,9 +772,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -803,9 +783,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -814,7 +794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -825,9 +805,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -836,9 +816,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -847,7 +827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -858,9 +838,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -869,9 +849,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -880,9 +860,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -891,7 +871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -902,9 +882,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -912,11 +892,10 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -925,7 +904,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -949,7 +928,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -960,7 +939,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -971,7 +950,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -982,7 +961,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1015,7 +994,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1026,7 +1005,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -1037,7 +1016,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -1048,7 +1027,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -1059,7 +1038,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -1070,7 +1049,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -1103,7 +1082,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1114,7 +1093,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
@@ -1125,7 +1104,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1136,7 +1115,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -1147,7 +1126,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -1158,7 +1137,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -1169,7 +1148,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -1180,7 +1159,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -1191,7 +1170,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1213,7 +1192,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
@@ -1235,7 +1214,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -1257,7 +1236,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -1268,7 +1247,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -1279,7 +1258,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -1290,7 +1269,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -1301,7 +1280,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
@@ -1312,7 +1291,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -1345,7 +1324,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
@@ -1356,7 +1335,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
@@ -1367,7 +1346,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -1378,7 +1357,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1389,7 +1368,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -1400,7 +1379,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -1411,7 +1390,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -1422,7 +1401,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -1433,7 +1412,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -1444,7 +1423,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -1455,7 +1434,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -1466,7 +1445,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -1477,7 +1456,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
@@ -1499,7 +1478,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
@@ -1510,7 +1489,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
@@ -1521,7 +1500,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
@@ -1532,7 +1511,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -1543,7 +1522,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -1554,7 +1533,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -1565,7 +1544,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -1587,7 +1566,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -1609,7 +1588,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
@@ -1620,7 +1599,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -1653,7 +1632,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -1664,7 +1643,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
@@ -1675,7 +1654,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
@@ -1686,7 +1665,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -1708,7 +1687,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -1719,7 +1698,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
@@ -1730,7 +1709,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
@@ -1741,7 +1720,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
@@ -1752,7 +1731,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
@@ -1763,7 +1742,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
@@ -1774,7 +1753,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
@@ -1785,7 +1764,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
@@ -1796,7 +1775,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
@@ -1807,7 +1786,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
@@ -1818,7 +1797,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
@@ -1829,7 +1808,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
@@ -1840,7 +1819,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
@@ -1862,7 +1841,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B101" t="s">
         <v>8</v>
@@ -1873,7 +1852,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
@@ -1895,7 +1874,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
@@ -1906,7 +1885,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -1917,7 +1896,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
@@ -1928,7 +1907,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
@@ -1939,7 +1918,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
@@ -1950,7 +1929,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
@@ -1961,7 +1940,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B110" t="s">
         <v>7</v>
@@ -1983,7 +1962,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
@@ -2005,7 +1984,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
@@ -2038,7 +2017,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B117" t="s">
         <v>8</v>
@@ -2049,7 +2028,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
@@ -2060,7 +2039,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B119" t="s">
         <v>8</v>
@@ -2071,7 +2050,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B120" t="s">
         <v>8</v>
@@ -2082,7 +2061,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B121" t="s">
         <v>7</v>
@@ -2093,7 +2072,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
@@ -2137,7 +2116,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B126" t="s">
         <v>9</v>
@@ -2148,7 +2127,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
@@ -2159,7 +2138,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
@@ -2170,7 +2149,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B129" t="s">
         <v>8</v>
@@ -2181,7 +2160,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
@@ -2203,7 +2182,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
@@ -2214,7 +2193,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B133" t="s">
         <v>8</v>
@@ -2236,7 +2215,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B135" t="s">
         <v>9</v>
@@ -2258,7 +2237,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B137" t="s">
         <v>9</v>
@@ -2269,7 +2248,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B138" t="s">
         <v>7</v>
@@ -2291,7 +2270,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B140" t="s">
         <v>9</v>
@@ -2302,7 +2281,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B141" t="s">
         <v>9</v>
@@ -2313,7 +2292,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B142" t="s">
         <v>8</v>
@@ -2324,7 +2303,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B143" t="s">
         <v>8</v>
@@ -2346,7 +2325,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
@@ -2368,7 +2347,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
@@ -2379,7 +2358,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
@@ -2390,7 +2369,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
         <v>9</v>
@@ -2401,7 +2380,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B150" t="s">
         <v>8</v>
@@ -2412,7 +2391,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B151" t="s">
         <v>9</v>
@@ -2423,7 +2402,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
@@ -2445,7 +2424,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B154" t="s">
         <v>9</v>
@@ -2456,7 +2435,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B155" t="s">
         <v>7</v>
@@ -2467,7 +2446,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B156" t="s">
         <v>8</v>
@@ -2478,7 +2457,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B157" t="s">
         <v>8</v>
@@ -2500,7 +2479,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B159" t="s">
         <v>9</v>
@@ -2522,7 +2501,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
@@ -2555,7 +2534,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
@@ -2566,7 +2545,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
@@ -2588,7 +2567,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
@@ -2599,7 +2578,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B168" t="s">
         <v>9</v>
@@ -2621,7 +2600,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B170" t="s">
         <v>7</v>
@@ -2632,7 +2611,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B171" t="s">
         <v>8</v>
@@ -2643,7 +2622,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B172" t="s">
         <v>7</v>
@@ -2654,7 +2633,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B173" t="s">
         <v>9</v>
@@ -2676,7 +2655,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B175" t="s">
         <v>9</v>
@@ -2687,7 +2666,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B176" t="s">
         <v>7</v>
@@ -2698,7 +2677,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B177" t="s">
         <v>9</v>
@@ -2709,7 +2688,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B178" t="s">
         <v>7</v>
@@ -2720,7 +2699,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B179" t="s">
         <v>8</v>
@@ -2731,7 +2710,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B180" t="s">
         <v>8</v>
@@ -2742,7 +2721,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B181" t="s">
         <v>9</v>
@@ -2753,7 +2732,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B182" t="s">
         <v>8</v>
@@ -2764,7 +2743,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B183" t="s">
         <v>7</v>
@@ -2775,7 +2754,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B184" t="s">
         <v>8</v>
@@ -2797,7 +2776,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B186" t="s">
         <v>9</v>
@@ -2808,7 +2787,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
@@ -2819,7 +2798,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B188" t="s">
         <v>9</v>
@@ -2830,7 +2809,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B189" t="s">
         <v>9</v>
@@ -2841,7 +2820,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B190" t="s">
         <v>8</v>
@@ -2852,7 +2831,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B191" t="s">
         <v>9</v>
@@ -2863,7 +2842,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B192" t="s">
         <v>9</v>
@@ -2874,7 +2853,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -2896,7 +2875,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B195" t="s">
         <v>9</v>
@@ -2907,7 +2886,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B196" t="s">
         <v>9</v>
@@ -2918,7 +2897,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -2940,7 +2919,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B199" t="s">
         <v>9</v>
@@ -2951,7 +2930,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B200" t="s">
         <v>9</v>
@@ -2962,7 +2941,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
@@ -2973,7 +2952,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B202" t="s">
         <v>7</v>
@@ -3006,7 +2985,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B205" t="s">
         <v>8</v>
@@ -3017,7 +2996,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B206" t="s">
         <v>8</v>
@@ -3050,7 +3029,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B209" t="s">
         <v>8</v>
@@ -3061,7 +3040,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B210" t="s">
         <v>7</v>
@@ -3072,7 +3051,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B211" t="s">
         <v>9</v>
@@ -3083,7 +3062,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B212" t="s">
         <v>7</v>
@@ -3094,7 +3073,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B213" t="s">
         <v>7</v>
@@ -3138,7 +3117,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B217" t="s">
         <v>9</v>
@@ -3149,7 +3128,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B218" t="s">
         <v>9</v>
@@ -3160,7 +3139,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B219" t="s">
         <v>7</v>
@@ -3171,7 +3150,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
@@ -3193,7 +3172,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
@@ -3215,7 +3194,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B224" t="s">
         <v>9</v>
@@ -3248,7 +3227,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B227" t="s">
         <v>8</v>
@@ -3270,7 +3249,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B229" t="s">
         <v>8</v>
@@ -3292,7 +3271,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B231" t="s">
         <v>8</v>
@@ -3314,7 +3293,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B233" t="s">
         <v>9</v>
@@ -3325,7 +3304,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B234" t="s">
         <v>9</v>
@@ -3336,7 +3315,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B235" t="s">
         <v>8</v>
@@ -3347,7 +3326,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B236" t="s">
         <v>9</v>

</xml_diff>